<commit_message>
remaining csv files from establishing and testing the comparable objects; when saving excel files to original back the related csv files disappear, but the excel file is still shown as different
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_EPICP_P1.xlsx
+++ b/rmonize/data_dictionary/DD_EPICP_P1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13071805-7099-4C33-9574-B5F8BA276141}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F061E7-E246-43D6-93F3-63C15214C4EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>index</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>TESTING</t>
+  </si>
+  <si>
+    <t>Testing 2</t>
   </si>
 </sst>
 </file>
@@ -765,7 +768,7 @@
   <dimension ref="A1:E250"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,6 +995,9 @@
       </c>
       <c r="B20" s="13">
         <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2005,6 +2011,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -2245,15 +2260,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
@@ -2266,6 +2272,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2282,12 +2296,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>